<commit_message>
Create .Net MVC Application for CI Platform
</commit_message>
<xml_diff>
--- a/DB/ci.xlsx
+++ b/DB/ci.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="112">
   <si>
     <t xml:space="preserve">Table : admin</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t xml:space="preserve">employee_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bigint</t>
   </si>
   <si>
     <t xml:space="preserve">manager_id</t>
@@ -754,14 +757,14 @@
   <dimension ref="A1:H151"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A146" activeCellId="0" sqref="A146"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.02"/>
@@ -1199,7 +1202,7 @@
         <v>34</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9" t="s">
@@ -1214,10 +1217,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5" t="s">
@@ -1232,10 +1235,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C25" s="5" t="n">
         <v>50</v>
@@ -1252,7 +1255,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>17</v>
@@ -1272,10 +1275,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5" t="s">
@@ -1290,10 +1293,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5" t="s">
@@ -1308,7 +1311,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>10</v>
@@ -1325,12 +1328,12 @@
         <v>14</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>10</v>
@@ -1347,15 +1350,15 @@
         <v>14</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C31" s="5" t="n">
         <v>30</v>
@@ -1372,7 +1375,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>17</v>
@@ -1392,7 +1395,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>10</v>
@@ -1409,7 +1412,7 @@
         <v>14</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1478,7 +1481,7 @@
     </row>
     <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1516,7 +1519,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>10</v>
@@ -1540,10 +1543,10 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C41" s="9" t="n">
         <v>100</v>
@@ -1560,10 +1563,10 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="9" t="s">
@@ -1578,10 +1581,10 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C43" s="9" t="n">
         <v>100</v>
@@ -1598,10 +1601,10 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="9" t="s">
@@ -1616,7 +1619,7 @@
     </row>
     <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1654,7 +1657,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>10</v>
@@ -1678,7 +1681,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>17</v>
@@ -1698,10 +1701,10 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5" t="s">
@@ -1716,10 +1719,10 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5" t="s">
@@ -1734,7 +1737,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>10</v>
@@ -1751,12 +1754,12 @@
         <v>14</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>10</v>
@@ -1773,12 +1776,12 @@
         <v>14</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>17</v>
@@ -1796,10 +1799,10 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5" t="s">
@@ -1812,10 +1815,10 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5" t="s">
@@ -1828,10 +1831,10 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="5" t="s">
@@ -1844,10 +1847,10 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C58" s="5" t="n">
         <v>5</v>
@@ -1862,7 +1865,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>10</v>
@@ -1878,10 +1881,10 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="5" t="s">
@@ -1894,7 +1897,7 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>10</v>
@@ -1909,12 +1912,12 @@
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="H61" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>10</v>
@@ -1927,12 +1930,12 @@
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
       <c r="H62" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>22</v>
@@ -1948,10 +1951,10 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5" t="s">
@@ -1964,10 +1967,10 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C65" s="5" t="n">
         <v>30</v>
@@ -1982,10 +1985,10 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="5" t="s">
@@ -2062,7 +2065,7 @@
     </row>
     <row r="71" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
@@ -2117,12 +2120,12 @@
         <v>14</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>10</v>
@@ -2139,12 +2142,12 @@
         <v>14</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>27</v>
@@ -2162,7 +2165,7 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>10</v>
@@ -2190,7 +2193,7 @@
     </row>
     <row r="78" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B78" s="12"/>
       <c r="C78" s="12"/>
@@ -2243,12 +2246,12 @@
         <v>14</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>10</v>
@@ -2265,12 +2268,12 @@
         <v>14</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>27</v>
@@ -2288,10 +2291,10 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="5" t="s">
@@ -2309,7 +2312,7 @@
     </row>
     <row r="85" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B85" s="12"/>
       <c r="C85" s="12"/>
@@ -2347,7 +2350,7 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>10</v>
@@ -2371,10 +2374,10 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C88" s="5" t="n">
         <v>50</v>
@@ -2391,7 +2394,7 @@
     </row>
     <row r="90" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -2429,7 +2432,7 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>10</v>
@@ -2453,10 +2456,10 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C93" s="5" t="n">
         <v>50</v>
@@ -2473,7 +2476,7 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>10</v>
@@ -2490,12 +2493,12 @@
         <v>14</v>
       </c>
       <c r="H94" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -2533,7 +2536,7 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>10</v>
@@ -2557,10 +2560,10 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C99" s="5" t="n">
         <v>50</v>
@@ -2586,7 +2589,7 @@
     </row>
     <row r="101" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -2624,7 +2627,7 @@
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>10</v>
@@ -2648,10 +2651,10 @@
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C104" s="5" t="n">
         <v>50</v>
@@ -2668,10 +2671,10 @@
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C105" s="5"/>
       <c r="D105" s="5" t="s">
@@ -2696,7 +2699,7 @@
     </row>
     <row r="107" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -2734,7 +2737,7 @@
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>10</v>
@@ -2758,10 +2761,10 @@
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B110" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C110" s="16" t="n">
         <v>200</v>
@@ -2778,7 +2781,7 @@
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B111" s="16" t="s">
         <v>10</v>
@@ -2795,7 +2798,7 @@
         <v>14</v>
       </c>
       <c r="H111" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2817,15 +2820,15 @@
         <v>14</v>
       </c>
       <c r="H112" s="16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B113" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C113" s="16"/>
       <c r="D113" s="16" t="s">
@@ -2840,7 +2843,7 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B114" s="16" t="s">
         <v>22</v>
@@ -2858,10 +2861,10 @@
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B115" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C115" s="16"/>
       <c r="D115" s="16" t="s">
@@ -2940,7 +2943,7 @@
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B120" s="12"/>
       <c r="C120" s="12"/>
@@ -2978,7 +2981,7 @@
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B122" s="5" t="s">
         <v>10</v>
@@ -2995,7 +2998,7 @@
         <v>14</v>
       </c>
       <c r="H122" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3017,12 +3020,12 @@
         <v>14</v>
       </c>
       <c r="H123" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B124" s="5" t="s">
         <v>10</v>
@@ -3039,12 +3042,12 @@
         <v>14</v>
       </c>
       <c r="H124" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B125" s="5" t="s">
         <v>27</v>
@@ -3062,10 +3065,10 @@
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C126" s="5"/>
       <c r="D126" s="5" t="s">
@@ -3080,7 +3083,7 @@
     </row>
     <row r="128" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B128" s="7"/>
       <c r="C128" s="7"/>
@@ -3118,7 +3121,7 @@
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B130" s="5" t="s">
         <v>10</v>
@@ -3142,10 +3145,10 @@
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B131" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C131" s="16"/>
       <c r="D131" s="16" t="s">
@@ -3177,12 +3180,12 @@
         <v>14</v>
       </c>
       <c r="H132" s="16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B133" s="16" t="s">
         <v>10</v>
@@ -3199,15 +3202,15 @@
         <v>14</v>
       </c>
       <c r="H133" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B134" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C134" s="16"/>
       <c r="D134" s="16" t="s">
@@ -3232,7 +3235,7 @@
     </row>
     <row r="136" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
@@ -3287,12 +3290,12 @@
         <v>14</v>
       </c>
       <c r="H138" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B139" s="5" t="s">
         <v>10</v>
@@ -3309,15 +3312,15 @@
         <v>14</v>
       </c>
       <c r="H139" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B140" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C140" s="16"/>
       <c r="D140" s="16" t="s">
@@ -3332,7 +3335,7 @@
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B141" s="16" t="s">
         <v>10</v>
@@ -3350,7 +3353,7 @@
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B142" s="16" t="s">
         <v>10</v>
@@ -3368,10 +3371,10 @@
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="16" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B143" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C143" s="16"/>
       <c r="D143" s="16" t="s">
@@ -3386,7 +3389,7 @@
     </row>
     <row r="145" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
@@ -3424,7 +3427,7 @@
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B147" s="5" t="s">
         <v>10</v>
@@ -3463,15 +3466,15 @@
         <v>14</v>
       </c>
       <c r="H148" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C149" s="5" t="n">
         <v>100</v>
@@ -3488,10 +3491,10 @@
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="16" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B150" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C150" s="16"/>
       <c r="D150" s="16" t="s">

</xml_diff>